<commit_message>
fix more complex merged table
</commit_message>
<xml_diff>
--- a/test/templates/test-tables-merged-line.xlsx
+++ b/test/templates/test-tables-merged-line.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1100023/Documents/xlsx-template-fork/test/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muyoungko/Documents/human/xlsx-template/test/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3E067B-D5C5-2245-8163-4BD4DC1C2F38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C6F1E79-12F1-7E40-860D-AF486ECCDF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>${table:scores.name}</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -35,18 +35,10 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>${table:scores.score}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>${score_first.name}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>${score_first.score}</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>${score_last.score}</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -61,6 +53,45 @@
   <si>
     <t>Name(2 col merged)</t>
     <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>${table:scores.score}</t>
+  </si>
+  <si>
+    <t>${score_first.score}</t>
+  </si>
+  <si>
+    <t>Second Table</t>
+  </si>
+  <si>
+    <t>${score2_first.name}</t>
+  </si>
+  <si>
+    <t>${table:scores2.name}</t>
+  </si>
+  <si>
+    <t>${score2_last.name}</t>
+  </si>
+  <si>
+    <t>${score2_last.score}</t>
+  </si>
+  <si>
+    <t>${table:scores2.score}</t>
+  </si>
+  <si>
+    <t>${score2_first.score}</t>
+  </si>
+  <si>
+    <t>${table:scores.extra}</t>
+  </si>
+  <si>
+    <t>${table:scores2.extra}</t>
   </si>
 </sst>
 </file>
@@ -117,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -200,8 +231,93 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -213,21 +329,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="dashed">
@@ -239,21 +342,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dashed">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="dashed">
@@ -265,11 +355,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="dashed">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -278,11 +400,13 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="dashed">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -291,34 +415,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="dashed">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -332,12 +449,60 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -350,50 +515,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="열어 본 하이퍼링크" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="열어 본 하이퍼링크" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="제목 1" xfId="1" builtinId="16"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="하이퍼링크" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -730,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:H15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="246" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="176" zoomScaleNormal="246" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -746,59 +881,140 @@
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20" thickBot="1">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:8" ht="20" thickBot="1">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="2:6" ht="14" thickTop="1"/>
-    <row r="4" spans="2:6" ht="14" thickBot="1">
+    <row r="3" spans="2:8" ht="14" thickTop="1"/>
+    <row r="4" spans="2:8" ht="14" thickBot="1">
       <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="H5" s="16"/>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6" t="s">
+    <row r="6" spans="2:8">
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="2:8" ht="14" thickBot="1">
+      <c r="B7" s="8" t="s">
         <v>4</v>
-      </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" spans="2:6" ht="14" thickBot="1">
-      <c r="B7" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="14"/>
+    </row>
+    <row r="10" spans="2:8" ht="20" thickBot="1">
+      <c r="B10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="14" thickTop="1"/>
+    <row r="12" spans="2:8" ht="14" thickBot="1">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="11"/>
+      <c r="E12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="21"/>
+      <c r="D13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="2:8" ht="14" thickBot="1">
+      <c r="B15" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="20">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:F5"/>
@@ -806,6 +1022,19 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:H15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>